<commit_message>
Completed design of MS2, not tested
</commit_message>
<xml_diff>
--- a/rtl/ms2/gnn.xlsx
+++ b/rtl/ms2/gnn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skmandal\Box\Sumit-PhD\ECE755\Project\GNN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/belatikar_wisc_edu/Documents/Spring'22/ECE755/Project/gnn-accelerator/rtl/ms2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEC2D2E-AA1D-4CDD-9207-33273EFFB3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="13_ncr:1_{3EEC2D2E-AA1D-4CDD-9207-33273EFFB3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CD154C5-3EAA-4587-9C7D-062E4EFF20CD}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="13344" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="few negative" sheetId="2" r:id="rId1"/>
@@ -227,6 +227,980 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>495120</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>29010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>524280</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>49890</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E89E639-8CED-4630-A3E2-63212775D39D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="5371920" y="390960"/>
+            <a:ext cx="29160" cy="20880"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E89E639-8CED-4630-A3E2-63212775D39D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5367600" y="386640"/>
+              <a:ext cx="37800" cy="29520"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219240</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95640</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="4" name="Ink 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C894FBFF-B1FB-4233-8A49-CE1DD6CA8E9C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="3876840" y="2990880"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="4" name="Ink 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C894FBFF-B1FB-4233-8A49-CE1DD6CA8E9C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3872520" y="2986560"/>
+              <a:ext cx="9000" cy="9000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>193560</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>140895</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>193920</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>141255</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E42F86C0-9E94-4A59-84EC-9895502D1739}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="4460760" y="2855520"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E42F86C0-9E94-4A59-84EC-9895502D1739}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4456440" y="2851200"/>
+              <a:ext cx="9000" cy="9000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>461280</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>51075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>461640</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>51435</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="15" name="Ink 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BDA8158-2DEF-4D49-B27F-40216CD90081}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="10824480" y="594000"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="15" name="Ink 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BDA8158-2DEF-4D49-B27F-40216CD90081}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10820160" y="589680"/>
+              <a:ext cx="9000" cy="9000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>364725</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>120810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>382725</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>128010</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="21" name="Ink 20">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5128D69D-8BA4-4590-B727-002DF73B09BB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="21386400" y="482760"/>
+            <a:ext cx="18000" cy="7200"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="21" name="Ink 20">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5128D69D-8BA4-4590-B727-002DF73B09BB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="21382080" y="478440"/>
+              <a:ext cx="26640" cy="15840"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>478125</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>111450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>507645</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>117930</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="22" name="Ink 21">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7F0D701-01FD-44E7-BAE8-B108AF03E833}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="21499800" y="473400"/>
+            <a:ext cx="29520" cy="6480"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="22" name="Ink 21">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7F0D701-01FD-44E7-BAE8-B108AF03E833}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="21495480" y="469080"/>
+              <a:ext cx="38160" cy="15120"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>370920</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>69780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>413400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>22005</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="23" name="Ink 22">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B371B342-6D2E-4D5F-A9E1-867E2092782C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="3418920" y="3689280"/>
+            <a:ext cx="42480" cy="133200"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="23" name="Ink 22">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B371B342-6D2E-4D5F-A9E1-867E2092782C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3414600" y="3684960"/>
+              <a:ext cx="51120" cy="141840"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>534000</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>61770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>539400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>89130</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="24" name="Ink 23">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF9C7003-F3DF-4966-A9DE-92DA7430915C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="5410800" y="423720"/>
+            <a:ext cx="5400" cy="27360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="24" name="Ink 23">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF9C7003-F3DF-4966-A9DE-92DA7430915C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5406480" y="419400"/>
+              <a:ext cx="14040" cy="36000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>482880</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>120090</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>493320</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>128010</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="27" name="Ink 26">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{664DF3F2-5AEF-4A50-9B97-F4AAD0C3DB5C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="5359680" y="482040"/>
+            <a:ext cx="10440" cy="7920"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="27" name="Ink 26">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{664DF3F2-5AEF-4A50-9B97-F4AAD0C3DB5C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5355360" y="477720"/>
+              <a:ext cx="19080" cy="16560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>432765</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>110010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>456165</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>121530</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="4" name="Ink 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B4D244A-0EFB-41B7-A729-ABA3FFB5A1FB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="21454440" y="471960"/>
+            <a:ext cx="23400" cy="11520"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="4" name="Ink 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B4D244A-0EFB-41B7-A729-ABA3FFB5A1FB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="21450120" y="467640"/>
+              <a:ext cx="32040" cy="20160"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T18:49:18.875"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">81 57 1848 0 0,'-5'-1'838'0'0,"1"-1"-1"0"0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1-1 1 0 0,1 1-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 1 0 0,-6-6-1 0 0,-13-8 1010 0 0,22 16-1989 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 219 0 0,4 0-5062 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink10.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T21:38:27.586"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">28 32 1096 0 0,'0'0'3201'0'0,"-28"0"-3369"0"0,28-4-312 0 0,0 1-2017 0 0,0 0 1345 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="442.63">28 32 3169 0 0,'36'-24'4905'0'0,"-37"24"-3113"0"0,-1 0-1208 0 0,0 0-200 0 0,0 0-152 0 0,1 0-248 0 0,1-4-992 0 0,0 1-2609 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T18:49:20.689"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 0 10938 0 0,'0'0'-1912'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T18:49:21.102"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">808 11 16259 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T18:56:29.111"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">306 339 3929 0 0,'0'0'5305'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T19:00:05.619"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">50 2 2192 0 0,'-4'2'10655'0'0,"-4"2"-8370"0"0,-1 0-292 0 0,3-1-1027 0 0,-4 1 6566 0 0,3-17-10026 0 0,1 8-2294 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink6.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T19:00:07.038"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">14 18 7562 0 0,'2'-4'536'0'0,"1"1"-696"0"0,1 3-192 0 0,1-4-80 0 0,7 4-33 0 0,0 0-263 0 0,0-3-608 0 0,-3 3-1329 0 0,0 0 705 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">14 18 14523 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">14 18 14523 0 0,'-14'-11'-968'0'0,"14"4"-1825"0"0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink7.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T21:27:41.867"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">117 0 2248 0 0,'-7'6'89'0'0,"-1"-1"-1"0"0,1 1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-5 12 1 0 0,3-2 125 0 0,1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-4 33 0 0 0,1 17 298 0 0,7-67-540 0 0,0 37-763 0 0,0 3-3157 0 0,0-37 3823 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink8.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T21:27:47.758"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">14 76 1816 0 0,'0'0'3369'0'0,"-1"-12"-3037"0"0,-6-39-76 0 0,5 39-730 0 0,0 14-567 0 0,0 10-2548 0 0,2-6 2920 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink9.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T21:27:48.305"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 7 0 0 0,'0'0'0'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="515.29">1 7 3617 0 0,'27'14'688'0'0,"-27"-17"776"0"0,-1-1-944 0 0,-1 1-104 0 0,-3-1 1 0 0,3 4-33 0 0,0-3-40 0 0,0-1-80 0 0,1 4-168 0 0</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -494,16 +1468,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A088C6-E004-4809-ACB0-707452AB5EBD}">
   <dimension ref="A1:AI26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="29" max="33" width="11.5703125" customWidth="1"/>
+    <col min="29" max="33" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -517,7 +1491,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>34</v>
       </c>
@@ -585,7 +1559,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -689,7 +1663,7 @@
         <v>-4188</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -793,7 +1767,7 @@
         <v>-4455</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -897,7 +1871,7 @@
         <v>-4587</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1001,7 +1975,7 @@
         <v>-4455</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K8" t="s">
         <v>4</v>
       </c>
@@ -1015,7 +1989,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K9" t="s">
         <v>5</v>
       </c>
@@ -1029,7 +2003,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K10" t="s">
         <v>6</v>
       </c>
@@ -1043,7 +2017,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K11" t="s">
         <v>7</v>
       </c>
@@ -1057,7 +2031,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K13" t="s">
         <v>8</v>
       </c>
@@ -1065,7 +2039,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K14" t="s">
         <v>9</v>
       </c>
@@ -1073,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K15" t="s">
         <v>10</v>
       </c>
@@ -1081,7 +2055,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K16" t="s">
         <v>11</v>
       </c>
@@ -1089,7 +2063,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K18" t="s">
         <v>12</v>
       </c>
@@ -1097,7 +2071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K19" t="s">
         <v>13</v>
       </c>
@@ -1105,7 +2079,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K20" t="s">
         <v>14</v>
       </c>
@@ -1113,7 +2087,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="21" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K21" t="s">
         <v>15</v>
       </c>
@@ -1121,7 +2095,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K23" t="s">
         <v>16</v>
       </c>
@@ -1129,7 +2103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K24" t="s">
         <v>17</v>
       </c>
@@ -1137,7 +2111,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="25" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K25" t="s">
         <v>32</v>
       </c>
@@ -1145,7 +2119,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K26" t="s">
         <v>33</v>
       </c>
@@ -1156,6 +2130,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1163,16 +2138,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AH11" sqref="AH11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="29" max="33" width="11.5703125" customWidth="1"/>
+    <col min="29" max="33" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1186,7 +2161,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>34</v>
       </c>
@@ -1254,7 +2229,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1358,7 +2333,7 @@
         <v>465750</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1462,7 +2437,7 @@
         <v>486000</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1566,7 +2541,7 @@
         <v>465750</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1670,7 +2645,7 @@
         <v>465750</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K8" t="s">
         <v>4</v>
       </c>
@@ -1684,7 +2659,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K9" t="s">
         <v>5</v>
       </c>
@@ -1698,7 +2673,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K10" t="s">
         <v>6</v>
       </c>
@@ -1712,7 +2687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K11" t="s">
         <v>7</v>
       </c>
@@ -1726,7 +2701,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K13" t="s">
         <v>8</v>
       </c>
@@ -1734,7 +2709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K14" t="s">
         <v>9</v>
       </c>
@@ -1742,7 +2717,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K15" t="s">
         <v>10</v>
       </c>
@@ -1750,7 +2725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K16" t="s">
         <v>11</v>
       </c>
@@ -1758,7 +2733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K18" t="s">
         <v>12</v>
       </c>
@@ -1766,7 +2741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K19" t="s">
         <v>13</v>
       </c>
@@ -1774,7 +2749,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K20" t="s">
         <v>14</v>
       </c>
@@ -1782,7 +2757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K21" t="s">
         <v>15</v>
       </c>
@@ -1790,7 +2765,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K23" t="s">
         <v>16</v>
       </c>
@@ -1798,7 +2773,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K24" t="s">
         <v>17</v>
       </c>
@@ -1806,7 +2781,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K25" t="s">
         <v>32</v>
       </c>
@@ -1814,7 +2789,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K26" t="s">
         <v>33</v>
       </c>
@@ -1824,6 +2799,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1831,16 +2807,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF04A0B2-8FF8-4FF6-9B25-F943D12D1C1E}">
   <dimension ref="A1:AI26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="U1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="29" max="33" width="11.5703125" customWidth="1"/>
+    <col min="29" max="33" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1854,7 +2830,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>34</v>
       </c>
@@ -1922,7 +2898,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2026,7 +3002,7 @@
         <v>-565248</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2130,7 +3106,7 @@
         <v>-589824</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2234,7 +3210,7 @@
         <v>-565248</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2338,7 +3314,7 @@
         <v>-565248</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K8" t="s">
         <v>4</v>
       </c>
@@ -2352,7 +3328,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K9" t="s">
         <v>5</v>
       </c>
@@ -2366,7 +3342,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K10" t="s">
         <v>6</v>
       </c>
@@ -2380,7 +3356,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K11" t="s">
         <v>7</v>
       </c>
@@ -2394,7 +3370,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K13" t="s">
         <v>8</v>
       </c>
@@ -2402,7 +3378,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K14" t="s">
         <v>9</v>
       </c>
@@ -2410,7 +3386,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K15" t="s">
         <v>10</v>
       </c>
@@ -2418,7 +3394,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="K16" t="s">
         <v>11</v>
       </c>
@@ -2426,7 +3402,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="18" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K18" t="s">
         <v>12</v>
       </c>
@@ -2434,7 +3410,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="19" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K19" t="s">
         <v>13</v>
       </c>
@@ -2442,7 +3418,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="20" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K20" t="s">
         <v>14</v>
       </c>
@@ -2450,7 +3426,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="21" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K21" t="s">
         <v>15</v>
       </c>
@@ -2458,7 +3434,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="23" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K23" t="s">
         <v>16</v>
       </c>
@@ -2466,7 +3442,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="24" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K24" t="s">
         <v>17</v>
       </c>
@@ -2474,7 +3450,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="25" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K25" t="s">
         <v>32</v>
       </c>
@@ -2482,7 +3458,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="26" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K26" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Verified design with given inputs and modified testbench to support edge cases
</commit_message>
<xml_diff>
--- a/rtl/ms2/gnn.xlsx
+++ b/rtl/ms2/gnn.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/belatikar_wisc_edu/Documents/Spring'22/ECE755/Project/gnn-accelerator/rtl/ms2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit\Box\Sumit-PhD\ECE755\Project\GNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="13_ncr:1_{3EEC2D2E-AA1D-4CDD-9207-33273EFFB3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CD154C5-3EAA-4587-9C7D-062E4EFF20CD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A2F6BF-717C-49DA-826D-2822032EB7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="13344" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="few negative" sheetId="2" r:id="rId1"/>
@@ -227,980 +227,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>495120</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>29010</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>524280</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>49890</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="2" name="Ink 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E89E639-8CED-4630-A3E2-63212775D39D}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="5371920" y="390960"/>
-            <a:ext cx="29160" cy="20880"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="2" name="Ink 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E89E639-8CED-4630-A3E2-63212775D39D}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="5367600" y="386640"/>
-              <a:ext cx="37800" cy="29520"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>219240</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>95280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>219600</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>95640</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="4" name="Ink 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C894FBFF-B1FB-4233-8A49-CE1DD6CA8E9C}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="3876840" y="2990880"/>
-            <a:ext cx="360" cy="360"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="4" name="Ink 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C894FBFF-B1FB-4233-8A49-CE1DD6CA8E9C}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3872520" y="2986560"/>
-              <a:ext cx="9000" cy="9000"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>193560</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>140895</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>193920</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>141255</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="5" name="Ink 4">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E42F86C0-9E94-4A59-84EC-9895502D1739}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="4460760" y="2855520"/>
-            <a:ext cx="360" cy="360"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="5" name="Ink 4">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E42F86C0-9E94-4A59-84EC-9895502D1739}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4456440" y="2851200"/>
-              <a:ext cx="9000" cy="9000"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>461280</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>51075</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>461640</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>51435</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="15" name="Ink 14">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BDA8158-2DEF-4D49-B27F-40216CD90081}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="10824480" y="594000"/>
-            <a:ext cx="360" cy="360"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="15" name="Ink 14">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BDA8158-2DEF-4D49-B27F-40216CD90081}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="10820160" y="589680"/>
-              <a:ext cx="9000" cy="9000"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>364725</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>120810</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>382725</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>128010</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="21" name="Ink 20">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5128D69D-8BA4-4590-B727-002DF73B09BB}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="21386400" y="482760"/>
-            <a:ext cx="18000" cy="7200"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="21" name="Ink 20">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5128D69D-8BA4-4590-B727-002DF73B09BB}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="21382080" y="478440"/>
-              <a:ext cx="26640" cy="15840"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>478125</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>111450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>507645</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>117930</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="22" name="Ink 21">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7F0D701-01FD-44E7-BAE8-B108AF03E833}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="21499800" y="473400"/>
-            <a:ext cx="29520" cy="6480"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="22" name="Ink 21">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7F0D701-01FD-44E7-BAE8-B108AF03E833}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="21495480" y="469080"/>
-              <a:ext cx="38160" cy="15120"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>370920</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>69780</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>413400</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>22005</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="23" name="Ink 22">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B371B342-6D2E-4D5F-A9E1-867E2092782C}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="3418920" y="3689280"/>
-            <a:ext cx="42480" cy="133200"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="23" name="Ink 22">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B371B342-6D2E-4D5F-A9E1-867E2092782C}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3414600" y="3684960"/>
-              <a:ext cx="51120" cy="141840"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>534000</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>61770</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>539400</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>89130</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="24" name="Ink 23">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF9C7003-F3DF-4966-A9DE-92DA7430915C}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="5410800" y="423720"/>
-            <a:ext cx="5400" cy="27360"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="24" name="Ink 23">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF9C7003-F3DF-4966-A9DE-92DA7430915C}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="5406480" y="419400"/>
-              <a:ext cx="14040" cy="36000"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>482880</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>120090</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>493320</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>128010</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="27" name="Ink 26">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{664DF3F2-5AEF-4A50-9B97-F4AAD0C3DB5C}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="5359680" y="482040"/>
-            <a:ext cx="10440" cy="7920"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="27" name="Ink 26">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{664DF3F2-5AEF-4A50-9B97-F4AAD0C3DB5C}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="5355360" y="477720"/>
-              <a:ext cx="19080" cy="16560"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>432765</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>110010</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>456165</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>121530</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="4" name="Ink 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B4D244A-0EFB-41B7-A729-ABA3FFB5A1FB}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="21454440" y="471960"/>
-            <a:ext cx="23400" cy="11520"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="4" name="Ink 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B4D244A-0EFB-41B7-A729-ABA3FFB5A1FB}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="21450120" y="467640"/>
-              <a:ext cx="32040" cy="20160"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
-          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
-          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T18:49:18.875"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.025" units="cm"/>
-      <inkml:brushProperty name="height" value="0.025" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">81 57 1848 0 0,'-5'-1'838'0'0,"1"-1"-1"0"0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1-1 1 0 0,1 1-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 1 0 0,-6-6-1 0 0,-13-8 1010 0 0,22 16-1989 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 219 0 0,4 0-5062 0 0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink10.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
-          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
-          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T21:38:27.586"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.025" units="cm"/>
-      <inkml:brushProperty name="height" value="0.025" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">28 32 1096 0 0,'0'0'3201'0'0,"-28"0"-3369"0"0,28-4-312 0 0,0 1-2017 0 0,0 0 1345 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="442.63">28 32 3169 0 0,'36'-24'4905'0'0,"-37"24"-3113"0"0,-1 0-1208 0 0,0 0-200 0 0,0 0-152 0 0,1 0-248 0 0,1-4-992 0 0,0 1-2609 0 0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
-          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
-          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T18:49:20.689"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.025" units="cm"/>
-      <inkml:brushProperty name="height" value="0.025" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 0 10938 0 0,'0'0'-1912'0'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
-          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
-          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T18:49:21.102"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.025" units="cm"/>
-      <inkml:brushProperty name="height" value="0.025" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">808 11 16259 0 0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
-          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
-          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T18:56:29.111"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.025" units="cm"/>
-      <inkml:brushProperty name="height" value="0.025" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">306 339 3929 0 0,'0'0'5305'0'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
-          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
-          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T19:00:05.619"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.025" units="cm"/>
-      <inkml:brushProperty name="height" value="0.025" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">50 2 2192 0 0,'-4'2'10655'0'0,"-4"2"-8370"0"0,-1 0-292 0 0,3-1-1027 0 0,-4 1 6566 0 0,3-17-10026 0 0,1 8-2294 0 0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink6.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
-          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
-          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T19:00:07.038"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.025" units="cm"/>
-      <inkml:brushProperty name="height" value="0.025" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">14 18 7562 0 0,'2'-4'536'0'0,"1"1"-696"0"0,1 3-192 0 0,1-4-80 0 0,7 4-33 0 0,0 0-263 0 0,0-3-608 0 0,-3 3-1329 0 0,0 0 705 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">14 18 14523 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">14 18 14523 0 0,'-14'-11'-968'0'0,"14"4"-1825"0"0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink7.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
-          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
-          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T21:27:41.867"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.025" units="cm"/>
-      <inkml:brushProperty name="height" value="0.025" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">117 0 2248 0 0,'-7'6'89'0'0,"-1"-1"-1"0"0,1 1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-5 12 1 0 0,3-2 125 0 0,1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-4 33 0 0 0,1 17 298 0 0,7-67-540 0 0,0 37-763 0 0,0 3-3157 0 0,0-37 3823 0 0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink8.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
-          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
-          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T21:27:47.758"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.025" units="cm"/>
-      <inkml:brushProperty name="height" value="0.025" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">14 76 1816 0 0,'0'0'3369'0'0,"-1"-12"-3037"0"0,-6-39-76 0 0,5 39-730 0 0,0 14-567 0 0,0 10-2548 0 0,2-6 2920 0 0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink9.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
-          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
-          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2022-03-04T21:27:48.305"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.025" units="cm"/>
-      <inkml:brushProperty name="height" value="0.025" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 7 0 0 0,'0'0'0'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="515.29">1 7 3617 0 0,'27'14'688'0'0,"-27"-17"776"0"0,-1-1-944 0 0,-1 1-104 0 0,-3-1 1 0 0,3 4-33 0 0,0-3-40 0 0,0-1-80 0 0,1 4-168 0 0</inkml:trace>
-</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1468,16 +494,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A088C6-E004-4809-ACB0-707452AB5EBD}">
   <dimension ref="A1:AI26"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="29" max="33" width="11.5546875" customWidth="1"/>
+    <col min="29" max="33" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1491,7 +517,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>34</v>
       </c>
@@ -1559,7 +585,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1663,7 +689,7 @@
         <v>-4188</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1767,7 +793,7 @@
         <v>-4455</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1871,7 +897,7 @@
         <v>-4587</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1975,7 +1001,7 @@
         <v>-4455</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K8" t="s">
         <v>4</v>
       </c>
@@ -1989,7 +1015,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K9" t="s">
         <v>5</v>
       </c>
@@ -2003,7 +1029,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K10" t="s">
         <v>6</v>
       </c>
@@ -2017,7 +1043,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K11" t="s">
         <v>7</v>
       </c>
@@ -2031,7 +1057,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K13" t="s">
         <v>8</v>
       </c>
@@ -2039,7 +1065,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K14" t="s">
         <v>9</v>
       </c>
@@ -2047,7 +1073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K15" t="s">
         <v>10</v>
       </c>
@@ -2055,7 +1081,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K16" t="s">
         <v>11</v>
       </c>
@@ -2063,7 +1089,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K18" t="s">
         <v>12</v>
       </c>
@@ -2071,7 +1097,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K19" t="s">
         <v>13</v>
       </c>
@@ -2079,7 +1105,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K20" t="s">
         <v>14</v>
       </c>
@@ -2087,7 +1113,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="21" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K21" t="s">
         <v>15</v>
       </c>
@@ -2095,7 +1121,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K23" t="s">
         <v>16</v>
       </c>
@@ -2103,7 +1129,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K24" t="s">
         <v>17</v>
       </c>
@@ -2111,7 +1137,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="25" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K25" t="s">
         <v>32</v>
       </c>
@@ -2119,7 +1145,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K26" t="s">
         <v>33</v>
       </c>
@@ -2130,7 +1156,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2138,16 +1163,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AH11" sqref="AH11"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="29" max="33" width="11.5546875" customWidth="1"/>
+    <col min="29" max="33" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -2161,7 +1186,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>34</v>
       </c>
@@ -2229,7 +1254,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2318,22 +1343,22 @@
       </c>
       <c r="AE3">
         <f t="shared" si="1"/>
-        <v>7425</v>
+        <v>8100</v>
       </c>
       <c r="AF3">
         <f t="shared" si="1"/>
-        <v>7425</v>
+        <v>8100</v>
       </c>
       <c r="AH3">
         <f>O3*AC3+O4*AD3+O5*AE3+O6*AF3</f>
-        <v>465750</v>
+        <v>486000</v>
       </c>
       <c r="AI3">
         <f>O8*AC3+O9*AD3+O10*AE3+O11*AF3</f>
-        <v>465750</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+        <v>486000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2437,7 +1462,7 @@
         <v>486000</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2490,12 +1515,12 @@
         <v>2700</v>
       </c>
       <c r="T5">
-        <f>J3*L18+J4*L19+L5*J20+J6*L21</f>
-        <v>2025</v>
+        <f>J3*L18+J4*L19+L5*L20+J6*L21</f>
+        <v>2700</v>
       </c>
       <c r="U5">
-        <f>J3*L23+J4*J24+J5*L25+J6*L26</f>
-        <v>2025</v>
+        <f>J3*L23+J4*L24+J5*L25+J6*L26</f>
+        <v>2700</v>
       </c>
       <c r="W5" t="s">
         <v>36</v>
@@ -2510,11 +1535,11 @@
       </c>
       <c r="Z5">
         <f t="shared" si="8"/>
-        <v>2025</v>
+        <v>2700</v>
       </c>
       <c r="AA5">
         <f t="shared" si="9"/>
-        <v>2025</v>
+        <v>2700</v>
       </c>
       <c r="AC5">
         <f>X3+X5+X6</f>
@@ -2526,22 +1551,22 @@
       </c>
       <c r="AE5">
         <f t="shared" si="11"/>
-        <v>7425</v>
+        <v>8100</v>
       </c>
       <c r="AF5">
         <f t="shared" si="11"/>
-        <v>7425</v>
+        <v>8100</v>
       </c>
       <c r="AH5">
         <f>O3*AC5+O4*AD5+O5*AE5+O6*AF5</f>
-        <v>465750</v>
+        <v>486000</v>
       </c>
       <c r="AI5">
         <f>O8*AC5+O9*AD5+O10*AE5+O11*AF5</f>
-        <v>465750</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+        <v>486000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2630,22 +1655,22 @@
       </c>
       <c r="AE6">
         <f t="shared" si="12"/>
-        <v>7425</v>
+        <v>8100</v>
       </c>
       <c r="AF6">
         <f t="shared" si="12"/>
-        <v>7425</v>
+        <v>8100</v>
       </c>
       <c r="AH6">
         <f>O3*AC6+O4*AD6+O5*AE6+O6*AF6</f>
-        <v>465750</v>
+        <v>486000</v>
       </c>
       <c r="AI6">
         <f>O8*AC6+O9*AD6+O10*AE6+O11*AF6</f>
-        <v>465750</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+        <v>486000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K8" t="s">
         <v>4</v>
       </c>
@@ -2659,7 +1684,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K9" t="s">
         <v>5</v>
       </c>
@@ -2673,7 +1698,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K10" t="s">
         <v>6</v>
       </c>
@@ -2687,7 +1712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K11" t="s">
         <v>7</v>
       </c>
@@ -2701,7 +1726,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K13" t="s">
         <v>8</v>
       </c>
@@ -2709,7 +1734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K14" t="s">
         <v>9</v>
       </c>
@@ -2717,7 +1742,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K15" t="s">
         <v>10</v>
       </c>
@@ -2725,7 +1750,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K16" t="s">
         <v>11</v>
       </c>
@@ -2733,7 +1758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K18" t="s">
         <v>12</v>
       </c>
@@ -2741,7 +1766,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K19" t="s">
         <v>13</v>
       </c>
@@ -2749,7 +1774,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K20" t="s">
         <v>14</v>
       </c>
@@ -2757,7 +1782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K21" t="s">
         <v>15</v>
       </c>
@@ -2765,7 +1790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K23" t="s">
         <v>16</v>
       </c>
@@ -2773,7 +1798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K24" t="s">
         <v>17</v>
       </c>
@@ -2781,7 +1806,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K25" t="s">
         <v>32</v>
       </c>
@@ -2789,7 +1814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K26" t="s">
         <v>33</v>
       </c>
@@ -2799,7 +1824,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2807,16 +1831,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF04A0B2-8FF8-4FF6-9B25-F943D12D1C1E}">
   <dimension ref="A1:AI26"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="29" max="33" width="11.5546875" customWidth="1"/>
+    <col min="29" max="33" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -2830,7 +1854,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>34</v>
       </c>
@@ -2898,7 +1922,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2987,22 +2011,22 @@
       </c>
       <c r="AE3">
         <f t="shared" si="1"/>
-        <v>8448</v>
+        <v>9216</v>
       </c>
       <c r="AF3">
         <f t="shared" si="1"/>
-        <v>8448</v>
+        <v>9216</v>
       </c>
       <c r="AH3">
         <f>O3*AC3+O4*AD3+O5*AE3+O6*AF3</f>
-        <v>-565248</v>
+        <v>-589824</v>
       </c>
       <c r="AI3">
         <f>O8*AC3+O9*AD3+O10*AE3+O11*AF3</f>
-        <v>-565248</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+        <v>-589824</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3106,7 +2130,7 @@
         <v>-589824</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -3159,12 +2183,12 @@
         <v>3072</v>
       </c>
       <c r="T5">
-        <f>J3*L18+J4*L19+L5*J20+J6*L21</f>
-        <v>2304</v>
+        <f>J3*L18+J4*L19+J5*L20+J6*L21</f>
+        <v>3072</v>
       </c>
       <c r="U5">
-        <f>J3*L23+J4*J24+J5*L25+J6*L26</f>
-        <v>2304</v>
+        <f>J3*L23+J4*L24+J5*L25+J6*L26</f>
+        <v>3072</v>
       </c>
       <c r="W5" t="s">
         <v>36</v>
@@ -3179,11 +2203,11 @@
       </c>
       <c r="Z5">
         <f t="shared" si="0"/>
-        <v>2304</v>
+        <v>3072</v>
       </c>
       <c r="AA5">
         <f t="shared" si="0"/>
-        <v>2304</v>
+        <v>3072</v>
       </c>
       <c r="AC5">
         <f>X3+X5+X6</f>
@@ -3195,22 +2219,22 @@
       </c>
       <c r="AE5">
         <f t="shared" si="8"/>
-        <v>8448</v>
+        <v>9216</v>
       </c>
       <c r="AF5">
         <f t="shared" si="8"/>
-        <v>8448</v>
+        <v>9216</v>
       </c>
       <c r="AH5">
         <f>O3*AC5+O4*AD5+O5*AE5+O6*AF5</f>
-        <v>-565248</v>
+        <v>-589824</v>
       </c>
       <c r="AI5">
         <f>O8*AC5+O9*AD5+O10*AE5+O11*AF5</f>
-        <v>-565248</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+        <v>-589824</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -3299,22 +2323,22 @@
       </c>
       <c r="AE6">
         <f t="shared" si="9"/>
-        <v>8448</v>
+        <v>9216</v>
       </c>
       <c r="AF6">
         <f t="shared" si="9"/>
-        <v>8448</v>
+        <v>9216</v>
       </c>
       <c r="AH6">
         <f>O3*AC6+O4*AD6+O5*AE6+O6*AF6</f>
-        <v>-565248</v>
+        <v>-589824</v>
       </c>
       <c r="AI6">
         <f>O8*AC6+O9*AD6+O10*AE6+O11*AF6</f>
-        <v>-565248</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+        <v>-589824</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K8" t="s">
         <v>4</v>
       </c>
@@ -3328,7 +2352,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K9" t="s">
         <v>5</v>
       </c>
@@ -3342,7 +2366,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K10" t="s">
         <v>6</v>
       </c>
@@ -3356,7 +2380,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K11" t="s">
         <v>7</v>
       </c>
@@ -3370,7 +2394,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K13" t="s">
         <v>8</v>
       </c>
@@ -3378,7 +2402,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K14" t="s">
         <v>9</v>
       </c>
@@ -3386,7 +2410,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K15" t="s">
         <v>10</v>
       </c>
@@ -3394,7 +2418,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="K16" t="s">
         <v>11</v>
       </c>
@@ -3402,7 +2426,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="18" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K18" t="s">
         <v>12</v>
       </c>
@@ -3410,7 +2434,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="19" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K19" t="s">
         <v>13</v>
       </c>
@@ -3418,7 +2442,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="20" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K20" t="s">
         <v>14</v>
       </c>
@@ -3426,7 +2450,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="21" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K21" t="s">
         <v>15</v>
       </c>
@@ -3434,7 +2458,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="23" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K23" t="s">
         <v>16</v>
       </c>
@@ -3442,7 +2466,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="24" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K24" t="s">
         <v>17</v>
       </c>
@@ -3450,7 +2474,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="25" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K25" t="s">
         <v>32</v>
       </c>
@@ -3458,7 +2482,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="26" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K26" t="s">
         <v>33</v>
       </c>

</xml_diff>